<commit_message>
agregar tipo de datos
Algunos, todavia faltan
</commit_message>
<xml_diff>
--- a/Planteamiento/Tablas Transportes.xlsx
+++ b/Planteamiento/Tablas Transportes.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKYNET\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JORGE\Documents\GitHub\Transportes\Planteamiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="750" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="111">
   <si>
     <t>Empresa</t>
   </si>
@@ -312,12 +312,57 @@
   </si>
   <si>
     <t>KM_Programacion</t>
+  </si>
+  <si>
+    <t>varchar(150)</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>numeric(18,2)</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">char(4) </t>
+  </si>
+  <si>
+    <t>char(4)</t>
+  </si>
+  <si>
+    <t>varchar(70)</t>
+  </si>
+  <si>
+    <t>varchar(15)</t>
+  </si>
+  <si>
+    <t>varchar(250)</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>char(5)</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>Id_Activo</t>
+  </si>
+  <si>
+    <t>char(8)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -457,11 +502,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -477,6 +575,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,618 +870,913 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4" style="28" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="4" style="20" customWidth="1"/>
+    <col min="13" max="13" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="N1" s="15"/>
+      <c r="P1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="17"/>
+      <c r="M2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="M3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="P4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="R5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="R6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="R7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="R8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="R9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="R10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="18"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B14" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="18"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="B16" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="18"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="18"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="O10" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="E24" s="12"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="H24" s="6"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="K24" s="12"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="N24" s="15"/>
+      <c r="P24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="H25" s="2"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="K25" s="2"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="N25" s="9"/>
+      <c r="P25" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="H26" s="2"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="K26" s="2"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="N26" s="9"/>
+      <c r="P26" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="K27" s="2"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="N27" s="9"/>
+      <c r="R27" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="H28" s="2"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="K28" s="2"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="N28" s="9"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D29" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="9"/>
+      <c r="F29" s="18"/>
+      <c r="M29" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="N29" s="9"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="9"/>
+      <c r="F30" s="18"/>
+      <c r="M30" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="N30" s="9"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="9"/>
+      <c r="F31" s="18"/>
+      <c r="M31" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
+      <c r="N31" s="9"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D32" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9"/>
+      <c r="F32" s="18"/>
+      <c r="M32" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
+      <c r="N32" s="9"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="1"/>
+      <c r="F33" s="22"/>
+      <c r="M33" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="N33" s="9"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="24"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="E41" s="12"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="H41" s="12"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K41" s="15"/>
+      <c r="L41" s="23"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="H42" s="2"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K42" s="9"/>
+      <c r="L42" s="18"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="E43" s="2"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="H43" s="2"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K43" s="9"/>
+      <c r="L43" s="18"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="E44" s="2"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="H44" s="2"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K44" s="9"/>
+      <c r="L44" s="18"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="E45" s="2"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="H45" s="2"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="13" t="s">
+      <c r="K45" s="9"/>
+      <c r="L45" s="18"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D46" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="E46" s="9"/>
+      <c r="F46" s="18"/>
+      <c r="J46" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
+      <c r="K46" s="9"/>
+      <c r="L46" s="18"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D47" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="9"/>
+      <c r="F47" s="18"/>
+      <c r="J47" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
+      <c r="K47" s="9"/>
+      <c r="L47" s="18"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D48" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="9"/>
+      <c r="F48" s="18"/>
+      <c r="J48" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="10" t="s">
+      <c r="K48" s="9"/>
+      <c r="L48" s="18"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D49" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="E49" s="9"/>
+      <c r="F49" s="18"/>
+      <c r="J49" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
+      <c r="K49" s="9"/>
+      <c r="L49" s="18"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1"/>
+      <c r="F50" s="22"/>
+      <c r="J50" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K50" s="1"/>
+      <c r="L50" s="22"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="5"/>
+      <c r="F60" s="21"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="1"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="1"/>
+      <c r="F61" s="22"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="1"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="1"/>
+      <c r="F62" s="22"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="1"/>
+      <c r="C63" s="18"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+      <c r="C64" s="18"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Avances Agente Empresa Aseguradora
</commit_message>
<xml_diff>
--- a/Planteamiento/Tablas Transportes.xlsx
+++ b/Planteamiento/Tablas Transportes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="2130" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="121">
   <si>
     <t>Activos</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>Secuencia</t>
+  </si>
+  <si>
+    <t>Nombre_Agente_Empresa_Aseguradora</t>
   </si>
 </sst>
 </file>
@@ -950,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:G12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1298,7 @@
         <v>48</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="21" t="s">
@@ -1701,7 +1704,7 @@
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="13" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="H53" s="18" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Dias Credito Proveedor y cliente
</commit_message>
<xml_diff>
--- a/Planteamiento/Tablas Transportes.xlsx
+++ b/Planteamiento/Tablas Transportes.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="128">
   <si>
     <t>Activos</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>varchar(10</t>
+  </si>
+  <si>
+    <t>Dias_Credito</t>
+  </si>
+  <si>
+    <t>numeric(18,0)</t>
   </si>
 </sst>
 </file>
@@ -1001,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,6 +1953,18 @@
       <c r="N63" s="1"/>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E64" s="31" t="s">
+        <v>127</v>
+      </c>
       <c r="F64" s="12"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>

</xml_diff>